<commit_message>
fix export and add jenis_shift
</commit_message>
<xml_diff>
--- a/directory/templates/template-absensi-harian.xlsx
+++ b/directory/templates/template-absensi-harian.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hrmis-master\directory\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444BE821-3C09-4295-A08F-3C39819C78F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EDBDC6-8D2F-4753-A629-5AA75C964633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6CD112B0-DD8C-4645-8F89-6FC547AE4A2B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Export Date : {app_export_date}</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>[jam_kerja] Jam</t>
+  </si>
+  <si>
+    <t>SHIFT</t>
+  </si>
+  <si>
+    <t>[jenis_shift]</t>
   </si>
 </sst>
 </file>
@@ -304,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -370,9 +376,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -390,6 +393,19 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -735,7 +751,7 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="B1" sqref="B1:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -749,25 +765,26 @@
     <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="2"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="35"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -783,19 +800,19 @@
     </row>
     <row r="2" spans="1:26" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="2"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="35"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -823,7 +840,7 @@
       <c r="K3" s="20"/>
       <c r="L3" s="20"/>
       <c r="M3" s="18"/>
-      <c r="N3" s="5"/>
+      <c r="N3" s="20"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
@@ -853,7 +870,7 @@
       <c r="K4" s="20"/>
       <c r="L4" s="20"/>
       <c r="M4" s="18"/>
-      <c r="N4" s="5"/>
+      <c r="N4" s="20"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
@@ -883,7 +900,7 @@
       <c r="K5" s="20"/>
       <c r="L5" s="20"/>
       <c r="M5" s="18"/>
-      <c r="N5" s="5"/>
+      <c r="N5" s="20"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
@@ -910,7 +927,7 @@
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
       <c r="M6" s="18"/>
-      <c r="N6" s="5"/>
+      <c r="N6" s="20"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
@@ -935,24 +952,26 @@
       <c r="D7" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="29" t="s">
+      <c r="G7" s="29"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="30"/>
-      <c r="K7" s="31"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="30"/>
       <c r="L7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="M7" s="18"/>
-      <c r="N7" s="3"/>
+      <c r="M7" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="31"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
@@ -971,7 +990,7 @@
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
-      <c r="E8" s="28"/>
+      <c r="E8" s="27"/>
       <c r="F8" s="14" t="s">
         <v>14</v>
       </c>
@@ -991,8 +1010,8 @@
         <v>16</v>
       </c>
       <c r="L8" s="24"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="7"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="32"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
@@ -1041,8 +1060,10 @@
       <c r="L9" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="M9" s="18"/>
-      <c r="N9" s="3"/>
+      <c r="M9" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="N9" s="31"/>
       <c r="O9" s="11"/>
       <c r="P9" s="11"/>
       <c r="Q9" s="11"/>
@@ -1070,7 +1091,7 @@
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
       <c r="M10" s="18"/>
-      <c r="N10" s="13"/>
+      <c r="N10" s="33"/>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
@@ -1088,9 +1109,10 @@
       <c r="M11" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="B1:M2"/>
     <mergeCell ref="L7:L8"/>
-    <mergeCell ref="B1:L2"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>

</xml_diff>

<commit_message>
fix export. add detail
</commit_message>
<xml_diff>
--- a/directory/templates/template-absensi-harian.xlsx
+++ b/directory/templates/template-absensi-harian.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hrmis-master\directory\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49EDBDC6-8D2F-4753-A629-5AA75C964633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C850F3B-2C0C-4675-BF3F-50245A7D2515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6CD112B0-DD8C-4645-8F89-6FC547AE4A2B}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
-  <si>
-    <t>Export Date : {app_export_date}</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>NO</t>
   </si>
@@ -42,9 +39,6 @@
     <t>[pegawai_nama]</t>
   </si>
   <si>
-    <t>SIMABSEN | ABSEN Hari {status}</t>
-  </si>
-  <si>
     <t>[nrp]</t>
   </si>
   <si>
@@ -93,9 +87,6 @@
     <t>[absen_id]</t>
   </si>
   <si>
-    <t>User : {user}</t>
-  </si>
-  <si>
     <t>[jam_kerja] Jam</t>
   </si>
   <si>
@@ -103,6 +94,9 @@
   </si>
   <si>
     <t>[jenis_shift]</t>
+  </si>
+  <si>
+    <t>HRMIS | Absen hari {status}</t>
   </si>
 </sst>
 </file>
@@ -310,7 +304,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -370,11 +364,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -393,19 +397,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -751,7 +742,7 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:M2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,21 +761,21 @@
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="35"/>
+      <c r="B1" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="25"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -800,19 +791,19 @@
     </row>
     <row r="2" spans="1:26" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="35"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="25"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -856,9 +847,7 @@
     </row>
     <row r="4" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="22" t="s">
-        <v>22</v>
-      </c>
+      <c r="B4" s="22"/>
       <c r="C4" s="6"/>
       <c r="D4" s="4"/>
       <c r="E4" s="6"/>
@@ -886,20 +875,34 @@
     </row>
     <row r="5" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="18"/>
+      <c r="C5" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="33"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="26" t="s">
+        <v>21</v>
+      </c>
       <c r="N5" s="20"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
@@ -916,17 +919,30 @@
     </row>
     <row r="6" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="M6" s="18"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
       <c r="N6" s="20"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
@@ -943,35 +959,43 @@
     </row>
     <row r="7" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="23" t="s">
+      <c r="B7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="29"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="M7" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="N7" s="31"/>
+      <c r="M7" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="23"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
@@ -987,31 +1011,19 @@
     </row>
     <row r="8" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="32"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="24"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
@@ -1026,44 +1038,7 @@
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="N9" s="31"/>
+      <c r="N9" s="3"/>
       <c r="O9" s="11"/>
       <c r="P9" s="11"/>
       <c r="Q9" s="11"/>
@@ -1078,20 +1053,8 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="33"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="13"/>
       <c r="O10" s="13"/>
       <c r="P10" s="13"/>
       <c r="Q10" s="13"/>
@@ -1110,15 +1073,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="M5:M6"/>
     <mergeCell ref="B1:M2"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:K5"/>
   </mergeCells>
   <conditionalFormatting sqref="H16:H100000">
     <cfRule type="expression" dxfId="1" priority="1">

</xml_diff>

<commit_message>
add unit_id for jadwal
</commit_message>
<xml_diff>
--- a/directory/templates/template-absensi-harian.xlsx
+++ b/directory/templates/template-absensi-harian.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hrmis-master\directory\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C850F3B-2C0C-4675-BF3F-50245A7D2515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEEB3A0C-0088-45D9-B8C1-BA8EE737AFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6CD112B0-DD8C-4645-8F89-6FC547AE4A2B}"/>
   </bookViews>
@@ -93,10 +93,10 @@
     <t>SHIFT</t>
   </si>
   <si>
-    <t>[jenis_shift]</t>
-  </si>
-  <si>
     <t>HRMIS | Absen hari {status}</t>
+  </si>
+  <si>
+    <t>[jadwal_nama]</t>
   </si>
 </sst>
 </file>
@@ -742,7 +742,7 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -762,7 +762,7 @@
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
@@ -993,7 +993,7 @@
         <v>20</v>
       </c>
       <c r="M7" s="21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N7" s="23"/>
       <c r="O7" s="3"/>

</xml_diff>

<commit_message>
using left join instead unit_id
</commit_message>
<xml_diff>
--- a/directory/templates/template-absensi-harian.xlsx
+++ b/directory/templates/template-absensi-harian.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hrmis-master\directory\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEEB3A0C-0088-45D9-B8C1-BA8EE737AFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A12FE6-E009-4D6B-8544-A8D77FF27F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6CD112B0-DD8C-4645-8F89-6FC547AE4A2B}"/>
   </bookViews>
@@ -742,7 +742,7 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -756,7 +756,7 @@
     <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
copy from hrmis gitlab
</commit_message>
<xml_diff>
--- a/directory/templates/template-absensi-harian.xlsx
+++ b/directory/templates/template-absensi-harian.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hrmis-master\directory\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\hrmis\directory\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188A7913-C716-4372-925C-7EE22B24F0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44092FB7-C709-42BB-88F6-370CC0A46E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6CD112B0-DD8C-4645-8F89-6FC547AE4A2B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>NO</t>
   </si>
@@ -72,9 +72,6 @@
     <t>[verifikasi_p]</t>
   </si>
   <si>
-    <t>[jam_kerja] Jam</t>
-  </si>
-  <si>
     <t>SHIFT</t>
   </si>
   <si>
@@ -115,6 +112,21 @@
   </si>
   <si>
     <t>HRMIS | Absen hari {tanggal_periode}</t>
+  </si>
+  <si>
+    <t>TANGGAL</t>
+  </si>
+  <si>
+    <t>[tanggal_absen]</t>
+  </si>
+  <si>
+    <t>[cek_waktu_masuk]</t>
+  </si>
+  <si>
+    <t>[cek_waktu_pulang]</t>
+  </si>
+  <si>
+    <t>[jam_kerja]</t>
   </si>
 </sst>
 </file>
@@ -215,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -288,17 +300,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -315,7 +316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -353,9 +354,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -377,64 +375,51 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -797,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D596E4BC-AD60-4373-9F8B-CF7958FFAB46}">
-  <dimension ref="A1:Z14"/>
+  <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -810,34 +795,35 @@
     <col min="4" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" customWidth="1"/>
+    <col min="10" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" customWidth="1"/>
     <col min="14" max="15" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="42"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
+      <c r="B1" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="16"/>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
@@ -849,23 +835,23 @@
     </row>
     <row r="2" spans="1:26" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="43"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="16"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
@@ -884,16 +870,16 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="18"/>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
       <c r="U3" s="5"/>
@@ -905,27 +891,27 @@
     </row>
     <row r="4" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
       <c r="U4" s="5"/>
@@ -937,14 +923,14 @@
     </row>
     <row r="5" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -953,11 +939,11 @@
       <c r="K5" s="14"/>
       <c r="L5" s="14"/>
       <c r="M5" s="14"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
@@ -981,11 +967,11 @@
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
@@ -997,41 +983,43 @@
     </row>
     <row r="7" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="E7" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="F7" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="29" t="s">
+      <c r="H7" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="29" t="s">
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="30"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="27" t="s">
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="O7" s="14"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
+      <c r="Q7" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="R7" s="32"/>
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
@@ -1043,35 +1031,35 @@
     </row>
     <row r="8" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
-      <c r="B8" s="28"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="28"/>
-      <c r="D8" s="24"/>
+      <c r="D8" s="26"/>
       <c r="E8" s="24"/>
       <c r="F8" s="24"/>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="24"/>
+      <c r="H8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="I8" s="29"/>
+      <c r="J8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="K8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="L8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="M8" s="29"/>
+      <c r="N8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="O8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="33"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
       <c r="U8" s="6"/>
@@ -1087,44 +1075,51 @@
         <v>2</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>17</v>
-      </c>
       <c r="E9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="7" t="s">
+      <c r="H9" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="I9" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="K9" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="L9" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="M9" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="N9" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
+      <c r="P9" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="R9" s="34"/>
       <c r="S9" s="10"/>
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
@@ -1150,9 +1145,9 @@
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
       <c r="O10" s="14"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
+      <c r="P10" s="35"/>
+      <c r="Q10" s="35"/>
+      <c r="R10" s="35"/>
       <c r="S10" s="12"/>
       <c r="T10" s="12"/>
       <c r="U10" s="12"/>
@@ -1163,31 +1158,31 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="P11" s="41"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
     </row>
     <row r="12" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="33"/>
+      <c r="D12" s="22"/>
     </row>
-    <row r="13" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="33"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="D14" s="34"/>
-    </row>
+    <row r="13" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="M7:M8"/>
+  <mergeCells count="15">
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="B1:N2"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="L7:O7"/>
+    <mergeCell ref="B1:Q2"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:C5">
     <cfRule type="expression" dxfId="3" priority="5">
@@ -1197,7 +1192,7 @@
       <formula>H18:H100009="Masuk"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H20:H100000 H17">
+  <conditionalFormatting sqref="H17 H20:H100000">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>H17:H100008="Pulang"</formula>
     </cfRule>

</xml_diff>